<commit_message>
Initial public release (#2)
* Update .gitignore

* Moved icon files

* Add Windows build script using PyInstaller

Introduces build.bat to automate building the executable for Windows using PyInstaller. The script includes necessary data and submodules, and provides user feedback during the build process.

* Fix metal leaching calculation

Refactored the metal leaching calculation in calcCosts() to compute the total mass of metal leached based on input composition and molar masses, improving cost normalization.

* Update Acid_properties.xlsx

* Update Acid_test.xlsx

* Refactor cost plotting to use stacked bar chart

Updated the pltCosts function to display reagent and heating costs per kg of metal leached as a single stacked bar chart instead of separate bar plots. This provides a clearer comparison of cost components across conditions.
</commit_message>
<xml_diff>
--- a/data/Acid_properties.xlsx
+++ b/data/Acid_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\ML-GUI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD797AF-1CA0-42B1-B1FF-0DCCC7A5BB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84581C3-8A8B-45E8-9B5C-AFC766CF0994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11110" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{D6E14713-EF62-40D5-A875-BAA3F7FAB13A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{D6E14713-EF62-40D5-A875-BAA3F7FAB13A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Acid</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>https://www.sigmaaldrich.com/PT/en/product/aldrich/w262706</t>
+  </si>
+  <si>
+    <t>https://www.chemanalyst.com/Pricing-data/oxalic-acid-1556</t>
   </si>
 </sst>
 </file>
@@ -625,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0684B1B-8EE6-404B-9FD1-135EF48961B7}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,14 +1093,24 @@
       <c r="L8">
         <v>1.9</v>
       </c>
+      <c r="M8">
+        <v>720</v>
+      </c>
       <c r="N8" s="1">
-        <v>80.400000000000006</v>
+        <f>M8*0.88*0.001</f>
+        <v>0.63360000000000005</v>
       </c>
       <c r="O8" s="5">
         <v>0.98</v>
       </c>
+      <c r="P8" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="Q8" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="R8" t="s">
+        <v>63</v>
       </c>
       <c r="S8">
         <v>0.18990000000000001</v>

</xml_diff>